<commit_message>
documentation revisited and changed to version 2
</commit_message>
<xml_diff>
--- a/Documentatie/Planning-RickBeniers-V1.xlsx
+++ b/Documentatie/Planning-RickBeniers-V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benie\Desktop\git-repos\GameDev-Periode1Project1Leerjaar3\2DTopDownScrollingShooter\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE55694F-2247-4007-A346-9CF8808A8B65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E34FBFAE-B744-42FE-8B06-8B941330D811}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9BD065F5-C26F-42C5-A094-E2ECB99C5A6F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="48">
   <si>
     <t>planning</t>
   </si>
@@ -277,6 +277,21 @@
   </si>
   <si>
     <t>C# binary database afgemaakt</t>
+  </si>
+  <si>
+    <t>Ambitie</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>speler kogels gemaakt, speler controle script afgemaakt</t>
+  </si>
+  <si>
+    <t>achtergrond geluiden deels geimplementeerd</t>
+  </si>
+  <si>
+    <t>begonnen aan Computer gestuurde speler scripten</t>
   </si>
 </sst>
 </file>
@@ -773,7 +788,7 @@
   <dimension ref="A2:J54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -783,6 +798,9 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -794,6 +812,9 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
@@ -941,7 +962,9 @@
         <v>22</v>
       </c>
       <c r="E12" s="10"/>
-      <c r="F12" s="3"/>
+      <c r="F12" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="17"/>
@@ -1024,7 +1047,9 @@
         <v>22</v>
       </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="3"/>
+      <c r="F18" s="3" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="17"/>
@@ -1050,7 +1075,9 @@
         <v>22</v>
       </c>
       <c r="E20" s="10"/>
-      <c r="F20" s="3"/>
+      <c r="F20" s="3" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="18"/>

</xml_diff>

<commit_message>
planning V2 made and GDD reworked for V2
</commit_message>
<xml_diff>
--- a/Documentatie/Planning-RickBeniers-V1.xlsx
+++ b/Documentatie/Planning-RickBeniers-V1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benie\Desktop\git-repos\GameDev-Periode1Project1Leerjaar3\2DTopDownScrollingShooter\Documentatie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3C6C81-E229-4431-923C-DB22CBC94453}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB77B23-55F1-4E9F-BD51-C3D7A0DC9FFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9BD065F5-C26F-42C5-A094-E2ECB99C5A6F}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
   <si>
     <t>planning</t>
   </si>
@@ -297,12 +297,6 @@
     <t>2 + 3 uur</t>
   </si>
   <si>
-    <t>project : doucumentatie V1 inleveren, trello bijwerken</t>
-  </si>
-  <si>
-    <t>GameDev : in-game winkel implementeren</t>
-  </si>
-  <si>
     <t>(Project :  documentatie bijwerken, OOP : Save/Load en highscore samenvoegen)</t>
   </si>
   <si>
@@ -330,9 +324,6 @@
     <t>GameDev : 5 extra eiland sprites implementeren</t>
   </si>
   <si>
-    <t>Versie 2 inleveren</t>
-  </si>
-  <si>
     <t>OOP : reflectie schrijven V2</t>
   </si>
   <si>
@@ -342,24 +333,9 @@
     <t>Testplan 1, Testen en Testen + opleveren</t>
   </si>
   <si>
-    <t>GameDev : activiteiten bepaald na TestPlan 2</t>
-  </si>
-  <si>
     <t>project : Testplan 2 uitvoeren &amp; planning deel 2 bepalen/schrijven</t>
   </si>
   <si>
-    <t>(Project : activiteiten bepaald na TestPlan 2 , OOP : activiteiten bepaald na TestPlan 2)</t>
-  </si>
-  <si>
-    <t>OOP : activiteiten bepaald na TestPlan 2</t>
-  </si>
-  <si>
-    <t>(GameDev : activiteiten bepaald na TestPlan 2)</t>
-  </si>
-  <si>
-    <t>project : activiteiten bepaald na TestPlan 2</t>
-  </si>
-  <si>
     <t>sprint 3 :</t>
   </si>
   <si>
@@ -373,6 +349,39 @@
   </si>
   <si>
     <t>(GameDev : Planning V2, GDD inleveren &amp; aanmerkingen stoter verwerken)</t>
+  </si>
+  <si>
+    <t>Versie 2 opleveren + documentatie</t>
+  </si>
+  <si>
+    <t>OOP : verslag afgemaakt en ingeleverd</t>
+  </si>
+  <si>
+    <t>(Project : sprite baseOfOperations implementeren, OOP : verder werken aan OPO)</t>
+  </si>
+  <si>
+    <t>GameDev : Object pooling(OPO) afmaken</t>
+  </si>
+  <si>
+    <t>OOP : base of operations werkend maken met de rest van de game</t>
+  </si>
+  <si>
+    <t>(GameDev : brandstof toevoegen als limiterende factor</t>
+  </si>
+  <si>
+    <t>project : brandstof werkend maken met de rest van de game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GameDev : planning V2 en GDD V2 ingeleverd </t>
+  </si>
+  <si>
+    <t>project : documentatie V1 inleveren, trello bijwerken</t>
+  </si>
+  <si>
+    <t>GameDev : in-game winkel onderzoeken hoe/wat</t>
+  </si>
+  <si>
+    <t>GameDev : Object pooling(OPO) onderzoeken hoe/wat</t>
   </si>
 </sst>
 </file>
@@ -556,6 +565,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -564,14 +581,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -888,8 +897,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24E12651-CE8A-405B-AD1B-293C86327EC9}">
   <dimension ref="A2:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,7 +941,7 @@
       <c r="C4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="D4" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="10"/>
@@ -953,7 +962,7 @@
       <c r="C5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="18"/>
+      <c r="D5" s="24"/>
       <c r="E5" s="11"/>
       <c r="F5" s="5"/>
     </row>
@@ -965,7 +974,7 @@
       <c r="C6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E6" s="10"/>
@@ -986,7 +995,7 @@
       <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="18"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="11"/>
       <c r="F7" s="5" t="s">
         <v>32</v>
@@ -1000,7 +1009,7 @@
       <c r="C8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="17" t="s">
+      <c r="D8" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E8" s="10"/>
@@ -1008,10 +1017,10 @@
         <v>33</v>
       </c>
       <c r="H8" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8" s="23"/>
-      <c r="J8" s="23"/>
+        <v>62</v>
+      </c>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
     </row>
     <row r="9" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13"/>
@@ -1021,7 +1030,7 @@
       <c r="C9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="24"/>
       <c r="E9" s="11"/>
       <c r="F9" s="5" t="s">
         <v>34</v>
@@ -1035,7 +1044,7 @@
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="10"/>
@@ -1043,10 +1052,10 @@
         <v>35</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
-      </c>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
+        <v>63</v>
+      </c>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
     </row>
     <row r="11" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="13"/>
@@ -1056,7 +1065,7 @@
       <c r="C11" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="18"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="11"/>
       <c r="F11" s="5" t="s">
         <v>36</v>
@@ -1070,7 +1079,7 @@
       <c r="C12" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="17" t="s">
+      <c r="D12" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E12" s="10"/>
@@ -1086,7 +1095,7 @@
       <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="18"/>
+      <c r="D13" s="24"/>
       <c r="E13" s="11"/>
       <c r="F13" s="5"/>
     </row>
@@ -1098,7 +1107,7 @@
       <c r="C14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="D14" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="10"/>
@@ -1113,7 +1122,7 @@
       <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="18"/>
+      <c r="D15" s="24"/>
       <c r="E15" s="11"/>
       <c r="F15" s="5" t="s">
         <v>41</v>
@@ -1127,7 +1136,7 @@
       <c r="C16" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D16" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E16" s="10"/>
@@ -1143,7 +1152,7 @@
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="18"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="11"/>
       <c r="F17" s="5"/>
     </row>
@@ -1155,7 +1164,7 @@
       <c r="C18" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D18" s="17" t="s">
+      <c r="D18" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="10"/>
@@ -1171,7 +1180,7 @@
       <c r="C19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="18"/>
+      <c r="D19" s="24"/>
       <c r="E19" s="11"/>
       <c r="F19" s="5"/>
     </row>
@@ -1183,7 +1192,7 @@
       <c r="C20" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D20" s="17" t="s">
+      <c r="D20" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E20" s="10"/>
@@ -1199,7 +1208,7 @@
       <c r="C21" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="18"/>
+      <c r="D21" s="24"/>
       <c r="E21" s="11"/>
       <c r="F21" s="5"/>
     </row>
@@ -1211,7 +1220,7 @@
       <c r="C22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D22" s="17" t="s">
+      <c r="D22" s="23" t="s">
         <v>21</v>
       </c>
       <c r="E22" s="10"/>
@@ -1227,7 +1236,7 @@
       <c r="C23" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D23" s="18"/>
+      <c r="D23" s="24"/>
       <c r="E23" s="11"/>
       <c r="F23" s="5"/>
     </row>
@@ -1239,7 +1248,7 @@
       <c r="C24" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D24" s="15"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="10"/>
       <c r="F24" s="3" t="s">
         <v>37</v>
@@ -1253,7 +1262,7 @@
       <c r="C25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="16"/>
+      <c r="D25" s="22"/>
       <c r="E25" s="11"/>
       <c r="F25" s="5"/>
     </row>
@@ -1263,9 +1272,9 @@
         <v>43739</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="15"/>
+        <v>60</v>
+      </c>
+      <c r="D26" s="21"/>
       <c r="E26" s="10"/>
       <c r="F26" s="3" t="s">
         <v>38</v>
@@ -1279,7 +1288,7 @@
       <c r="C27" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="16"/>
+      <c r="D27" s="22"/>
       <c r="E27" s="11"/>
       <c r="F27" s="5"/>
     </row>
@@ -1303,13 +1312,13 @@
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B31" s="19">
+      <c r="B31" s="15">
         <v>43745</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D31" s="15"/>
+      <c r="D31" s="21"/>
       <c r="E31" s="10"/>
       <c r="F31" s="3"/>
     </row>
@@ -1320,40 +1329,44 @@
       <c r="C32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="16"/>
+      <c r="D32" s="22"/>
       <c r="E32" s="11"/>
       <c r="F32" s="5"/>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B33" s="19">
+      <c r="B33" s="15">
         <v>43746</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D33" s="15"/>
+        <v>65</v>
+      </c>
+      <c r="D33" s="21"/>
       <c r="E33" s="10"/>
-      <c r="F33" s="3"/>
+      <c r="F33" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="34" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C34" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="D34" s="22"/>
+      <c r="E34" s="11"/>
+      <c r="F34" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="5"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B35" s="19">
+      <c r="B35" s="15">
         <v>43747</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D35" s="15"/>
+        <v>75</v>
+      </c>
+      <c r="D35" s="21"/>
       <c r="E35" s="10"/>
       <c r="F35" s="3"/>
     </row>
@@ -1364,40 +1377,40 @@
       <c r="C36" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="22"/>
       <c r="E36" s="11"/>
       <c r="F36" s="5"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B37" s="19">
+      <c r="B37" s="15">
         <v>43748</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="15"/>
+        <v>76</v>
+      </c>
+      <c r="D37" s="21"/>
       <c r="E37" s="10"/>
       <c r="F37" s="3"/>
     </row>
     <row r="38" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B38" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="16"/>
+        <v>49</v>
+      </c>
+      <c r="D38" s="22"/>
       <c r="E38" s="11"/>
       <c r="F38" s="5"/>
     </row>
     <row r="39" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B39" s="19">
+      <c r="B39" s="15">
         <v>43752</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="D39" s="21"/>
       <c r="E39" s="10"/>
       <c r="F39" s="3"/>
     </row>
@@ -1408,18 +1421,18 @@
       <c r="C40" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D40" s="16"/>
+      <c r="D40" s="22"/>
       <c r="E40" s="11"/>
       <c r="F40" s="5"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B41" s="19">
+      <c r="B41" s="15">
         <v>43753</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D41" s="15"/>
+        <v>52</v>
+      </c>
+      <c r="D41" s="21"/>
       <c r="E41" s="10"/>
       <c r="F41" s="3"/>
     </row>
@@ -1428,20 +1441,20 @@
         <v>48</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D42" s="16"/>
+        <v>53</v>
+      </c>
+      <c r="D42" s="22"/>
       <c r="E42" s="11"/>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B43" s="19">
+      <c r="B43" s="15">
         <v>43754</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="15"/>
+        <v>55</v>
+      </c>
+      <c r="D43" s="21"/>
       <c r="E43" s="10"/>
       <c r="F43" s="3"/>
     </row>
@@ -1452,40 +1465,40 @@
       <c r="C44" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D44" s="16"/>
+      <c r="D44" s="22"/>
       <c r="E44" s="11"/>
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B45" s="19">
+      <c r="B45" s="15">
         <v>43755</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D45" s="15"/>
+        <v>54</v>
+      </c>
+      <c r="D45" s="21"/>
       <c r="E45" s="10"/>
       <c r="F45" s="3"/>
     </row>
     <row r="46" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="D46" s="16"/>
+        <v>56</v>
+      </c>
+      <c r="D46" s="22"/>
       <c r="E46" s="11"/>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B47" s="19">
+      <c r="B47" s="15">
         <v>43759</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" s="15"/>
+        <v>57</v>
+      </c>
+      <c r="D47" s="21"/>
       <c r="E47" s="10"/>
       <c r="F47" s="3"/>
     </row>
@@ -1496,18 +1509,18 @@
       <c r="C48" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D48" s="16"/>
+      <c r="D48" s="22"/>
       <c r="E48" s="11"/>
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B49" s="19">
+      <c r="B49" s="15">
         <v>43760</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D49" s="15"/>
+        <v>58</v>
+      </c>
+      <c r="D49" s="21"/>
       <c r="E49" s="10"/>
       <c r="F49" s="3"/>
     </row>
@@ -1516,20 +1529,20 @@
         <v>48</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" s="16"/>
+        <v>59</v>
+      </c>
+      <c r="D50" s="22"/>
       <c r="E50" s="11"/>
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B51" s="19">
+      <c r="B51" s="15">
         <v>43761</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D51" s="15"/>
+        <v>61</v>
+      </c>
+      <c r="D51" s="21"/>
       <c r="E51" s="10"/>
       <c r="F51" s="3"/>
     </row>
@@ -1540,40 +1553,40 @@
       <c r="C52" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="16"/>
+      <c r="D52" s="22"/>
       <c r="E52" s="11"/>
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B53" s="19">
+      <c r="B53" s="15">
         <v>43762</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D53" s="15"/>
+        <v>77</v>
+      </c>
+      <c r="D53" s="21"/>
       <c r="E53" s="10"/>
       <c r="F53" s="3"/>
     </row>
     <row r="54" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D54" s="16"/>
+        <v>69</v>
+      </c>
+      <c r="D54" s="22"/>
       <c r="E54" s="11"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B55" s="19">
+      <c r="B55" s="15">
         <v>43766</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D55" s="21"/>
+        <v>70</v>
+      </c>
+      <c r="D55" s="17"/>
       <c r="E55" s="9"/>
       <c r="F55" s="3"/>
     </row>
@@ -1584,18 +1597,18 @@
       <c r="C56" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D56" s="22"/>
+      <c r="D56" s="18"/>
       <c r="E56" s="8"/>
       <c r="F56" s="5"/>
     </row>
     <row r="57" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B57" s="19">
+      <c r="B57" s="15">
         <v>43767</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D57" s="21"/>
+        <v>71</v>
+      </c>
+      <c r="D57" s="17"/>
       <c r="E57" s="9"/>
       <c r="F57" s="3"/>
     </row>
@@ -1604,20 +1617,20 @@
         <v>48</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D58" s="22"/>
+        <v>72</v>
+      </c>
+      <c r="D58" s="18"/>
       <c r="E58" s="8"/>
       <c r="F58" s="5"/>
     </row>
     <row r="59" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B59" s="19">
+      <c r="B59" s="15">
         <v>43768</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D59" s="21"/>
+        <v>73</v>
+      </c>
+      <c r="D59" s="17"/>
       <c r="E59" s="9"/>
       <c r="F59" s="3"/>
     </row>
@@ -1628,18 +1641,18 @@
       <c r="C60" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D60" s="22"/>
+      <c r="D60" s="18"/>
       <c r="E60" s="8"/>
       <c r="F60" s="5"/>
     </row>
     <row r="61" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B61" s="19">
+      <c r="B61" s="15">
         <v>43769</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D61" s="21"/>
+        <v>64</v>
+      </c>
+      <c r="D61" s="17"/>
       <c r="E61" s="9"/>
       <c r="F61" s="3"/>
     </row>
@@ -1648,18 +1661,18 @@
       <c r="C62" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="22"/>
+      <c r="D62" s="18"/>
       <c r="E62" s="8"/>
       <c r="F62" s="5"/>
     </row>
     <row r="63" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B63" s="19">
+      <c r="B63" s="15">
         <v>43770</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D63" s="21"/>
+        <v>67</v>
+      </c>
+      <c r="D63" s="17"/>
       <c r="E63" s="9"/>
       <c r="F63" s="3"/>
     </row>
@@ -1668,7 +1681,7 @@
       <c r="C64" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D64" s="22"/>
+      <c r="D64" s="18"/>
       <c r="E64" s="8"/>
       <c r="F64" s="5"/>
     </row>
@@ -1676,22 +1689,34 @@
       <c r="C65" s="10"/>
     </row>
     <row r="66" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C66" s="20"/>
+      <c r="C66" s="16"/>
     </row>
     <row r="67" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C67" s="20"/>
+      <c r="C67" s="16"/>
     </row>
     <row r="68" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C68" s="20"/>
+      <c r="C68" s="16"/>
     </row>
     <row r="69" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C69" s="20"/>
+      <c r="C69" s="16"/>
     </row>
     <row r="70" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C70" s="20"/>
+      <c r="C70" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="D31:D32"/>
+    <mergeCell ref="D33:D34"/>
+    <mergeCell ref="D35:D36"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="D47:D48"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="D51:D52"/>
     <mergeCell ref="D26:D27"/>
     <mergeCell ref="D4:D5"/>
     <mergeCell ref="D6:D7"/>
@@ -1704,18 +1729,6 @@
     <mergeCell ref="D20:D21"/>
     <mergeCell ref="D22:D23"/>
     <mergeCell ref="D24:D25"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="D31:D32"/>
-    <mergeCell ref="D33:D34"/>
-    <mergeCell ref="D35:D36"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="D47:D48"/>
-    <mergeCell ref="D49:D50"/>
-    <mergeCell ref="D51:D52"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>